<commit_message>
fix more VII typos
</commit_message>
<xml_diff>
--- a/inc/flattened/createYaml/VII-splitstems.xlsx
+++ b/inc/flattened/createYaml/VII-splitstems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherhammerly/giellalt/lang-ciw/inc/flattened/createYaml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13BA18B-9A2C-F947-8348-909D63EDDD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45680558-6F55-B34E-ACD0-38392E495B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27340" yWindow="4100" windowWidth="27320" windowHeight="14860" xr2:uid="{F60773C9-26C0-414F-936B-204C5C4D934C}"/>
+    <workbookView xWindow="-27320" yWindow="5060" windowWidth="27320" windowHeight="14860" activeTab="1" xr2:uid="{F60773C9-26C0-414F-936B-204C5C4D934C}"/>
   </bookViews>
   <sheets>
     <sheet name="VII_IND" sheetId="1" r:id="rId1"/>
@@ -483,9 +483,6 @@
     <t>ate&gt;&gt;sininigoban</t>
   </si>
   <si>
-    <t>ates&gt;&gt;ininigobaniin</t>
-  </si>
-  <si>
     <t>ate&gt;&gt;gobanen</t>
   </si>
   <si>
@@ -1111,6 +1108,9 @@
   </si>
   <si>
     <t>bangisin&gt;&gt;0</t>
+  </si>
+  <si>
+    <t>ate&gt;&gt;sininigobaniin</t>
   </si>
 </sst>
 </file>
@@ -1470,8 +1470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA193F61-3C0D-9941-81CC-6F6AD6C92B40}">
   <dimension ref="A1:I257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B251" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H195" sqref="H195"/>
+    <sheetView topLeftCell="A152" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D162" sqref="D162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1535,7 +1535,7 @@
         <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2391,7 +2391,7 @@
         <v>36</v>
       </c>
       <c r="H34" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -3247,7 +3247,7 @@
         <v>36</v>
       </c>
       <c r="H66" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
@@ -3912,7 +3912,7 @@
         <v>143</v>
       </c>
       <c r="I91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
@@ -3967,7 +3967,7 @@
         <v>145</v>
       </c>
       <c r="I93" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
@@ -4022,7 +4022,7 @@
         <v>147</v>
       </c>
       <c r="I95" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
@@ -4074,10 +4074,10 @@
         <v>37</v>
       </c>
       <c r="H97" t="s">
-        <v>149</v>
+        <v>358</v>
       </c>
       <c r="I97" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
@@ -4103,7 +4103,7 @@
         <v>36</v>
       </c>
       <c r="H98" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
@@ -4152,7 +4152,7 @@
         <v>36</v>
       </c>
       <c r="H100" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
@@ -4201,7 +4201,7 @@
         <v>37</v>
       </c>
       <c r="H102" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
@@ -4250,7 +4250,7 @@
         <v>37</v>
       </c>
       <c r="H104" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
@@ -4851,7 +4851,7 @@
         <v>36</v>
       </c>
       <c r="H130" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
@@ -4877,7 +4877,7 @@
         <v>36</v>
       </c>
       <c r="H131" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
@@ -4903,7 +4903,7 @@
         <v>36</v>
       </c>
       <c r="H132" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.2">
@@ -4929,7 +4929,7 @@
         <v>36</v>
       </c>
       <c r="H133" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
@@ -4955,7 +4955,7 @@
         <v>37</v>
       </c>
       <c r="H134" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
@@ -4981,7 +4981,7 @@
         <v>37</v>
       </c>
       <c r="H135" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
@@ -5007,7 +5007,7 @@
         <v>37</v>
       </c>
       <c r="H136" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
@@ -5033,7 +5033,7 @@
         <v>37</v>
       </c>
       <c r="H137" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
@@ -5059,7 +5059,7 @@
         <v>36</v>
       </c>
       <c r="H138" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
@@ -5085,10 +5085,10 @@
         <v>36</v>
       </c>
       <c r="H139" t="s">
+        <v>160</v>
+      </c>
+      <c r="I139" t="s">
         <v>161</v>
-      </c>
-      <c r="I139" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
@@ -5114,7 +5114,7 @@
         <v>36</v>
       </c>
       <c r="H140" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
@@ -5140,10 +5140,10 @@
         <v>36</v>
       </c>
       <c r="H141" t="s">
+        <v>163</v>
+      </c>
+      <c r="I141" t="s">
         <v>164</v>
-      </c>
-      <c r="I141" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
@@ -5169,7 +5169,7 @@
         <v>37</v>
       </c>
       <c r="H142" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
@@ -5195,10 +5195,10 @@
         <v>37</v>
       </c>
       <c r="H143" t="s">
+        <v>166</v>
+      </c>
+      <c r="I143" t="s">
         <v>167</v>
-      </c>
-      <c r="I143" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
@@ -5224,7 +5224,7 @@
         <v>37</v>
       </c>
       <c r="H144" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
@@ -5250,10 +5250,10 @@
         <v>37</v>
       </c>
       <c r="H145" t="s">
+        <v>169</v>
+      </c>
+      <c r="I145" t="s">
         <v>170</v>
-      </c>
-      <c r="I145" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
@@ -5279,7 +5279,7 @@
         <v>36</v>
       </c>
       <c r="H146" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
@@ -5305,7 +5305,7 @@
         <v>36</v>
       </c>
       <c r="H147" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
@@ -5331,7 +5331,7 @@
         <v>36</v>
       </c>
       <c r="H148" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
@@ -5357,7 +5357,7 @@
         <v>36</v>
       </c>
       <c r="H149" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
@@ -5383,7 +5383,7 @@
         <v>37</v>
       </c>
       <c r="H150" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
@@ -5409,7 +5409,7 @@
         <v>37</v>
       </c>
       <c r="H151" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
@@ -5435,7 +5435,7 @@
         <v>37</v>
       </c>
       <c r="H152" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
@@ -5461,7 +5461,7 @@
         <v>37</v>
       </c>
       <c r="H153" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
@@ -5487,7 +5487,7 @@
         <v>36</v>
       </c>
       <c r="H154" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.2">
@@ -5513,10 +5513,10 @@
         <v>36</v>
       </c>
       <c r="H155" t="s">
+        <v>179</v>
+      </c>
+      <c r="I155" t="s">
         <v>180</v>
-      </c>
-      <c r="I155" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
@@ -5542,7 +5542,7 @@
         <v>36</v>
       </c>
       <c r="H156" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
@@ -5568,10 +5568,10 @@
         <v>36</v>
       </c>
       <c r="H157" t="s">
+        <v>182</v>
+      </c>
+      <c r="I157" t="s">
         <v>183</v>
-      </c>
-      <c r="I157" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
@@ -5597,7 +5597,7 @@
         <v>37</v>
       </c>
       <c r="H158" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
@@ -5623,10 +5623,10 @@
         <v>37</v>
       </c>
       <c r="H159" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I159" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
@@ -5652,7 +5652,7 @@
         <v>37</v>
       </c>
       <c r="H160" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
@@ -5678,10 +5678,10 @@
         <v>37</v>
       </c>
       <c r="H161" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I161" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
@@ -5707,7 +5707,7 @@
         <v>36</v>
       </c>
       <c r="H162" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
@@ -5733,7 +5733,7 @@
         <v>36</v>
       </c>
       <c r="H163" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.2">
@@ -5759,7 +5759,7 @@
         <v>36</v>
       </c>
       <c r="H164" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
@@ -5785,7 +5785,7 @@
         <v>36</v>
       </c>
       <c r="H165" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.2">
@@ -5811,7 +5811,7 @@
         <v>37</v>
       </c>
       <c r="H166" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.2">
@@ -5837,7 +5837,7 @@
         <v>37</v>
       </c>
       <c r="H167" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.2">
@@ -5863,7 +5863,7 @@
         <v>37</v>
       </c>
       <c r="H168" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.2">
@@ -5889,7 +5889,7 @@
         <v>37</v>
       </c>
       <c r="H169" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.2">
@@ -5915,7 +5915,7 @@
         <v>36</v>
       </c>
       <c r="H170" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.2">
@@ -5941,10 +5941,10 @@
         <v>36</v>
       </c>
       <c r="H171" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I171" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.2">
@@ -5970,7 +5970,7 @@
         <v>36</v>
       </c>
       <c r="H172" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.2">
@@ -5996,10 +5996,10 @@
         <v>36</v>
       </c>
       <c r="H173" t="s">
+        <v>200</v>
+      </c>
+      <c r="I173" t="s">
         <v>201</v>
-      </c>
-      <c r="I173" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.2">
@@ -6025,7 +6025,7 @@
         <v>37</v>
       </c>
       <c r="H174" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.2">
@@ -6051,10 +6051,10 @@
         <v>37</v>
       </c>
       <c r="H175" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I175" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
@@ -6080,7 +6080,7 @@
         <v>37</v>
       </c>
       <c r="H176" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
@@ -6106,10 +6106,10 @@
         <v>37</v>
       </c>
       <c r="H177" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I177" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
@@ -6135,7 +6135,7 @@
         <v>36</v>
       </c>
       <c r="H178" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.2">
@@ -6161,7 +6161,7 @@
         <v>36</v>
       </c>
       <c r="H179" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
@@ -6187,7 +6187,7 @@
         <v>36</v>
       </c>
       <c r="H180" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.2">
@@ -6213,7 +6213,7 @@
         <v>36</v>
       </c>
       <c r="H181" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.2">
@@ -6239,7 +6239,7 @@
         <v>37</v>
       </c>
       <c r="H182" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.2">
@@ -6265,7 +6265,7 @@
         <v>37</v>
       </c>
       <c r="H183" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.2">
@@ -6291,7 +6291,7 @@
         <v>37</v>
       </c>
       <c r="H184" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.2">
@@ -6317,7 +6317,7 @@
         <v>37</v>
       </c>
       <c r="H185" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.2">
@@ -6343,7 +6343,7 @@
         <v>36</v>
       </c>
       <c r="H186" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.2">
@@ -6369,10 +6369,10 @@
         <v>36</v>
       </c>
       <c r="H187" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I187" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.2">
@@ -6398,7 +6398,7 @@
         <v>36</v>
       </c>
       <c r="H188" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.2">
@@ -6424,10 +6424,10 @@
         <v>36</v>
       </c>
       <c r="H189" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I189" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.2">
@@ -6453,7 +6453,7 @@
         <v>37</v>
       </c>
       <c r="H190" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.2">
@@ -6479,10 +6479,10 @@
         <v>37</v>
       </c>
       <c r="H191" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I191" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.2">
@@ -6508,7 +6508,7 @@
         <v>37</v>
       </c>
       <c r="H192" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.2">
@@ -6534,10 +6534,10 @@
         <v>37</v>
       </c>
       <c r="H193" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I193" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.2">
@@ -6563,7 +6563,7 @@
         <v>36</v>
       </c>
       <c r="H194" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.2">
@@ -6589,7 +6589,7 @@
         <v>36</v>
       </c>
       <c r="H195" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.2">
@@ -6615,7 +6615,7 @@
         <v>36</v>
       </c>
       <c r="H196" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.2">
@@ -6641,7 +6641,7 @@
         <v>36</v>
       </c>
       <c r="H197" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.2">
@@ -6667,7 +6667,7 @@
         <v>37</v>
       </c>
       <c r="H198" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.2">
@@ -6693,7 +6693,7 @@
         <v>37</v>
       </c>
       <c r="H199" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.2">
@@ -6719,7 +6719,7 @@
         <v>37</v>
       </c>
       <c r="H200" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.2">
@@ -6745,7 +6745,7 @@
         <v>37</v>
       </c>
       <c r="H201" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.2">
@@ -6771,7 +6771,7 @@
         <v>36</v>
       </c>
       <c r="H202" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.2">
@@ -6797,10 +6797,10 @@
         <v>36</v>
       </c>
       <c r="H203" t="s">
+        <v>234</v>
+      </c>
+      <c r="I203" t="s">
         <v>235</v>
-      </c>
-      <c r="I203" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.2">
@@ -6826,7 +6826,7 @@
         <v>36</v>
       </c>
       <c r="H204" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.2">
@@ -6852,10 +6852,10 @@
         <v>36</v>
       </c>
       <c r="H205" t="s">
+        <v>237</v>
+      </c>
+      <c r="I205" t="s">
         <v>238</v>
-      </c>
-      <c r="I205" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.2">
@@ -6881,7 +6881,7 @@
         <v>37</v>
       </c>
       <c r="H206" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.2">
@@ -6907,10 +6907,10 @@
         <v>37</v>
       </c>
       <c r="H207" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I207" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.2">
@@ -6936,7 +6936,7 @@
         <v>37</v>
       </c>
       <c r="H208" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.2">
@@ -6962,10 +6962,10 @@
         <v>37</v>
       </c>
       <c r="H209" t="s">
+        <v>243</v>
+      </c>
+      <c r="I209" t="s">
         <v>244</v>
-      </c>
-      <c r="I209" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.2">
@@ -6991,7 +6991,7 @@
         <v>36</v>
       </c>
       <c r="H210" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.2">
@@ -7017,7 +7017,7 @@
         <v>36</v>
       </c>
       <c r="H211" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.2">
@@ -7043,7 +7043,7 @@
         <v>36</v>
       </c>
       <c r="H212" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.2">
@@ -7069,7 +7069,7 @@
         <v>36</v>
       </c>
       <c r="H213" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.2">
@@ -7095,7 +7095,7 @@
         <v>37</v>
       </c>
       <c r="H214" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.2">
@@ -7121,7 +7121,7 @@
         <v>37</v>
       </c>
       <c r="H215" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.2">
@@ -7147,7 +7147,7 @@
         <v>37</v>
       </c>
       <c r="H216" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.2">
@@ -7173,7 +7173,7 @@
         <v>37</v>
       </c>
       <c r="H217" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.2">
@@ -7199,7 +7199,7 @@
         <v>36</v>
       </c>
       <c r="H218" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.2">
@@ -7225,10 +7225,10 @@
         <v>36</v>
       </c>
       <c r="H219" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I219" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.2">
@@ -7254,7 +7254,7 @@
         <v>36</v>
       </c>
       <c r="H220" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.2">
@@ -7280,10 +7280,10 @@
         <v>36</v>
       </c>
       <c r="H221" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I221" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.2">
@@ -7309,7 +7309,7 @@
         <v>37</v>
       </c>
       <c r="H222" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.2">
@@ -7335,10 +7335,10 @@
         <v>37</v>
       </c>
       <c r="H223" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I223" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.2">
@@ -7364,7 +7364,7 @@
         <v>37</v>
       </c>
       <c r="H224" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.2">
@@ -7390,10 +7390,10 @@
         <v>37</v>
       </c>
       <c r="H225" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I225" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.2">
@@ -7419,7 +7419,7 @@
         <v>36</v>
       </c>
       <c r="H226" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.2">
@@ -7445,7 +7445,7 @@
         <v>36</v>
       </c>
       <c r="H227" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.2">
@@ -7471,7 +7471,7 @@
         <v>36</v>
       </c>
       <c r="H228" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.2">
@@ -7497,7 +7497,7 @@
         <v>36</v>
       </c>
       <c r="H229" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.2">
@@ -7523,7 +7523,7 @@
         <v>37</v>
       </c>
       <c r="H230" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.2">
@@ -7549,7 +7549,7 @@
         <v>37</v>
       </c>
       <c r="H231" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.2">
@@ -7575,7 +7575,7 @@
         <v>37</v>
       </c>
       <c r="H232" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.2">
@@ -7601,7 +7601,7 @@
         <v>37</v>
       </c>
       <c r="H233" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.2">
@@ -8169,8 +8169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10602B5-8061-9841-B1CF-59F4D777D95C}">
   <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView topLeftCell="B111" zoomScale="141" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="141" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8238,7 +8238,7 @@
         <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -8264,7 +8264,7 @@
         <v>36</v>
       </c>
       <c r="H3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -8290,7 +8290,7 @@
         <v>37</v>
       </c>
       <c r="H4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -8316,7 +8316,7 @@
         <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -8342,7 +8342,7 @@
         <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -8368,7 +8368,7 @@
         <v>36</v>
       </c>
       <c r="H7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -8394,7 +8394,7 @@
         <v>37</v>
       </c>
       <c r="H8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -8420,7 +8420,7 @@
         <v>37</v>
       </c>
       <c r="H9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -8446,7 +8446,7 @@
         <v>36</v>
       </c>
       <c r="H10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -8472,7 +8472,7 @@
         <v>36</v>
       </c>
       <c r="H11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -8498,7 +8498,7 @@
         <v>37</v>
       </c>
       <c r="H12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -8524,7 +8524,7 @@
         <v>37</v>
       </c>
       <c r="H13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -8576,7 +8576,7 @@
         <v>36</v>
       </c>
       <c r="H15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -8654,7 +8654,7 @@
         <v>36</v>
       </c>
       <c r="H18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -8680,7 +8680,7 @@
         <v>36</v>
       </c>
       <c r="H19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -8706,7 +8706,7 @@
         <v>37</v>
       </c>
       <c r="H20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -8732,7 +8732,7 @@
         <v>37</v>
       </c>
       <c r="H21" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -8758,7 +8758,7 @@
         <v>36</v>
       </c>
       <c r="H22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -8784,7 +8784,7 @@
         <v>36</v>
       </c>
       <c r="H23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -8810,7 +8810,7 @@
         <v>37</v>
       </c>
       <c r="H24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -8836,7 +8836,7 @@
         <v>37</v>
       </c>
       <c r="H25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -8862,7 +8862,7 @@
         <v>36</v>
       </c>
       <c r="H26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -8888,7 +8888,7 @@
         <v>36</v>
       </c>
       <c r="H27" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -8914,7 +8914,7 @@
         <v>37</v>
       </c>
       <c r="H28" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -8940,7 +8940,7 @@
         <v>37</v>
       </c>
       <c r="H29" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -9070,7 +9070,7 @@
         <v>36</v>
       </c>
       <c r="H34" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -9096,7 +9096,7 @@
         <v>36</v>
       </c>
       <c r="H35" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -9122,7 +9122,7 @@
         <v>37</v>
       </c>
       <c r="H36" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -9148,7 +9148,7 @@
         <v>37</v>
       </c>
       <c r="H37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -9174,7 +9174,7 @@
         <v>36</v>
       </c>
       <c r="H38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -9200,7 +9200,7 @@
         <v>36</v>
       </c>
       <c r="H39" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -9226,7 +9226,7 @@
         <v>37</v>
       </c>
       <c r="H40" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -9252,7 +9252,7 @@
         <v>37</v>
       </c>
       <c r="H41" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -9278,7 +9278,7 @@
         <v>36</v>
       </c>
       <c r="H42" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -9304,7 +9304,7 @@
         <v>36</v>
       </c>
       <c r="H43" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -9376,7 +9376,7 @@
         <v>36</v>
       </c>
       <c r="H46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -9402,7 +9402,7 @@
         <v>36</v>
       </c>
       <c r="H47" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -9428,7 +9428,7 @@
         <v>37</v>
       </c>
       <c r="H48" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -9454,7 +9454,7 @@
         <v>37</v>
       </c>
       <c r="H49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -9480,7 +9480,7 @@
         <v>36</v>
       </c>
       <c r="H50" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -9529,7 +9529,7 @@
         <v>37</v>
       </c>
       <c r="H52" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -9854,7 +9854,7 @@
         <v>36</v>
       </c>
       <c r="H66" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -9880,7 +9880,7 @@
         <v>36</v>
       </c>
       <c r="H67" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -9906,7 +9906,7 @@
         <v>37</v>
       </c>
       <c r="H68" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -9932,7 +9932,7 @@
         <v>37</v>
       </c>
       <c r="H69" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -9958,7 +9958,7 @@
         <v>36</v>
       </c>
       <c r="H70" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -9984,7 +9984,7 @@
         <v>36</v>
       </c>
       <c r="H71" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -10010,7 +10010,7 @@
         <v>37</v>
       </c>
       <c r="H72" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -10036,7 +10036,7 @@
         <v>37</v>
       </c>
       <c r="H73" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
@@ -10062,7 +10062,7 @@
         <v>36</v>
       </c>
       <c r="H74" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
@@ -10088,7 +10088,7 @@
         <v>36</v>
       </c>
       <c r="H75" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -10114,7 +10114,7 @@
         <v>37</v>
       </c>
       <c r="H76" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -10140,7 +10140,7 @@
         <v>37</v>
       </c>
       <c r="H77" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -10166,7 +10166,7 @@
         <v>36</v>
       </c>
       <c r="H78" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -10192,7 +10192,7 @@
         <v>36</v>
       </c>
       <c r="H79" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -10218,7 +10218,7 @@
         <v>37</v>
       </c>
       <c r="H80" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -10244,7 +10244,7 @@
         <v>37</v>
       </c>
       <c r="H81" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -10270,7 +10270,7 @@
         <v>36</v>
       </c>
       <c r="H82" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -10296,7 +10296,7 @@
         <v>36</v>
       </c>
       <c r="H83" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -10322,7 +10322,7 @@
         <v>37</v>
       </c>
       <c r="H84" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -10348,7 +10348,7 @@
         <v>37</v>
       </c>
       <c r="H85" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -10374,7 +10374,7 @@
         <v>36</v>
       </c>
       <c r="H86" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -10400,7 +10400,7 @@
         <v>36</v>
       </c>
       <c r="H87" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -10426,7 +10426,7 @@
         <v>37</v>
       </c>
       <c r="H88" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -10452,7 +10452,7 @@
         <v>37</v>
       </c>
       <c r="H89" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -10478,7 +10478,7 @@
         <v>36</v>
       </c>
       <c r="H90" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -10504,7 +10504,7 @@
         <v>36</v>
       </c>
       <c r="H91" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -10530,7 +10530,7 @@
         <v>37</v>
       </c>
       <c r="H92" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -10556,7 +10556,7 @@
         <v>37</v>
       </c>
       <c r="H93" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -10582,7 +10582,7 @@
         <v>36</v>
       </c>
       <c r="H94" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -10608,7 +10608,7 @@
         <v>36</v>
       </c>
       <c r="H95" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -10634,7 +10634,7 @@
         <v>37</v>
       </c>
       <c r="H96" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
@@ -10660,7 +10660,7 @@
         <v>37</v>
       </c>
       <c r="H97" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -10686,7 +10686,7 @@
         <v>36</v>
       </c>
       <c r="H98" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
@@ -10712,7 +10712,7 @@
         <v>36</v>
       </c>
       <c r="H99" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
@@ -10738,7 +10738,7 @@
         <v>37</v>
       </c>
       <c r="H100" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -10764,7 +10764,7 @@
         <v>37</v>
       </c>
       <c r="H101" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
@@ -10790,7 +10790,7 @@
         <v>36</v>
       </c>
       <c r="H102" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
@@ -10816,7 +10816,7 @@
         <v>36</v>
       </c>
       <c r="H103" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
@@ -10842,7 +10842,7 @@
         <v>37</v>
       </c>
       <c r="H104" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
@@ -10868,7 +10868,7 @@
         <v>37</v>
       </c>
       <c r="H105" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
@@ -10894,7 +10894,7 @@
         <v>36</v>
       </c>
       <c r="H106" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
@@ -10920,7 +10920,7 @@
         <v>36</v>
       </c>
       <c r="H107" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
@@ -10946,7 +10946,7 @@
         <v>37</v>
       </c>
       <c r="H108" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
@@ -10972,7 +10972,7 @@
         <v>37</v>
       </c>
       <c r="H109" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
@@ -10998,7 +10998,7 @@
         <v>36</v>
       </c>
       <c r="H110" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
@@ -11024,7 +11024,7 @@
         <v>36</v>
       </c>
       <c r="H111" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
@@ -11050,7 +11050,7 @@
         <v>37</v>
       </c>
       <c r="H112" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
@@ -11076,7 +11076,7 @@
         <v>37</v>
       </c>
       <c r="H113" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
@@ -11102,7 +11102,7 @@
         <v>36</v>
       </c>
       <c r="H114" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
@@ -11151,7 +11151,7 @@
         <v>37</v>
       </c>
       <c r="H116" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -11627,18 +11627,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11661,6 +11661,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A50646E-DC1C-4D16-AC23-4B244D7154EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0CFA308-43F1-499A-8049-AAB3DA408682}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -11675,12 +11683,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A50646E-DC1C-4D16-AC23-4B244D7154EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update VAI spilts and rules
</commit_message>
<xml_diff>
--- a/inc/flattened/createYaml/VII-splitstems.xlsx
+++ b/inc/flattened/createYaml/VII-splitstems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherhammerly/giellalt/lang-ciw/inc/flattened/createYaml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45680558-6F55-B34E-ACD0-38392E495B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A2CEB6-F487-0D47-B09F-FFAF457E442E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27320" yWindow="5060" windowWidth="27320" windowHeight="14860" activeTab="1" xr2:uid="{F60773C9-26C0-414F-936B-204C5C4D934C}"/>
   </bookViews>
@@ -8169,8 +8169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10602B5-8061-9841-B1CF-59F4D777D95C}">
   <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="141" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="141" workbookViewId="0">
+      <selection activeCell="H95" sqref="H95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update the notes file, fix issues with VAIs that caused yaml fails
</commit_message>
<xml_diff>
--- a/inc/flattened/createYaml/VII-splitstems.xlsx
+++ b/inc/flattened/createYaml/VII-splitstems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherhammerly/giellalt/lang-ciw/inc/flattened/createYaml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A2CEB6-F487-0D47-B09F-FFAF457E442E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4005572E-287E-A64C-AAE3-B9F5E252F0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27320" yWindow="5060" windowWidth="27320" windowHeight="14860" activeTab="1" xr2:uid="{F60773C9-26C0-414F-936B-204C5C4D934C}"/>
+    <workbookView xWindow="-27320" yWindow="5060" windowWidth="27320" windowHeight="14860" xr2:uid="{F60773C9-26C0-414F-936B-204C5C4D934C}"/>
   </bookViews>
   <sheets>
     <sheet name="VII_IND" sheetId="1" r:id="rId1"/>
@@ -1470,8 +1470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA193F61-3C0D-9941-81CC-6F6AD6C92B40}">
   <dimension ref="A1:I257"/>
   <sheetViews>
-    <sheetView topLeftCell="A152" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D162" sqref="D162"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D226" sqref="D226:H233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8169,8 +8169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10602B5-8061-9841-B1CF-59F4D777D95C}">
   <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="141" workbookViewId="0">
-      <selection activeCell="H95" sqref="H95"/>
+    <sheetView topLeftCell="A22" zoomScale="141" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11462,6 +11462,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EDA4FEBE11D32545B6C4D443ADFB229A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fa29c2c3225ad03fb09b8df90fa91a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b103a3be-6c61-44b0-93c5-2b779aa38a01" xmlns:ns3="56612388-9f28-4625-93a0-6879c02082d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2c16c82533632c11d7fcceef7f9e9ea5" ns2:_="" ns3:_="">
     <xsd:import namespace="b103a3be-6c61-44b0-93c5-2b779aa38a01"/>
@@ -11626,22 +11641,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0CFA308-43F1-499A-8049-AAB3DA408682}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="56612388-9f28-4625-93a0-6879c02082d6"/>
+    <ds:schemaRef ds:uri="b103a3be-6c61-44b0-93c5-2b779aa38a01"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A50646E-DC1C-4D16-AC23-4B244D7154EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CADB2AF-8FF4-4CD3-86AB-7AA08F493F37}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11658,29 +11683,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A50646E-DC1C-4D16-AC23-4B244D7154EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0CFA308-43F1-499A-8049-AAB3DA408682}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="56612388-9f28-4625-93a0-6879c02082d6"/>
-    <ds:schemaRef ds:uri="b103a3be-6c61-44b0-93c5-2b779aa38a01"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>